<commit_message>
Updated example service import spreadsheet (#60)
</commit_message>
<xml_diff>
--- a/public/downloads/services_import_example.xlsx
+++ b/public/downloads/services_import_example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -67,6 +67,12 @@
     <t>referral_method</t>
   </si>
   <si>
+    <t>show_referral_disclaimer</t>
+  </si>
+  <si>
+    <t>referral_button_text</t>
+  </si>
+  <si>
     <t>referral_email</t>
   </si>
   <si>
@@ -97,7 +103,7 @@
     <t>criteria_other</t>
   </si>
   <si>
-    <t>fda66c8e-1086-4820-9e54-95538a3a7026</t>
+    <t>b2c3845a-1652-4049-be0e-7d133c531160</t>
   </si>
   <si>
     <t>00c05ada-1fa3-48a8-aa47-df15b5d07114</t>
@@ -109,7 +115,7 @@
     <t>One of: service, activity, club, group</t>
   </si>
   <si>
-    <t>inactive</t>
+    <t>One of: inactive, active</t>
   </si>
   <si>
     <t>Introduction text</t>
@@ -191,6 +197,12 @@
   </si>
   <si>
     <t>One of: internal, external, none</t>
+  </si>
+  <si>
+    <t>Redundant field - must be 1</t>
+  </si>
+  <si>
+    <t>Redundant field - enter "Connect"</t>
   </si>
   <si>
     <r>
@@ -533,17 +545,17 @@
     <col customWidth="1" min="15" max="15" width="18.14"/>
     <col customWidth="1" min="16" max="16" width="24.71"/>
     <col customWidth="1" min="17" max="17" width="49.57"/>
-    <col customWidth="1" min="18" max="18" width="38.29"/>
-    <col customWidth="1" min="19" max="19" width="48.29"/>
-    <col customWidth="1" min="20" max="20" width="21.43"/>
-    <col customWidth="1" min="21" max="21" width="29.14"/>
-    <col customWidth="1" min="22" max="22" width="26.43"/>
-    <col customWidth="1" min="23" max="23" width="28.71"/>
-    <col customWidth="1" min="24" max="24" width="25.71"/>
-    <col customWidth="1" min="25" max="25" width="22.29"/>
-    <col customWidth="1" min="26" max="26" width="25.29"/>
-    <col customWidth="1" min="27" max="27" width="29.86"/>
-    <col customWidth="1" min="28" max="28" width="63.71"/>
+    <col customWidth="1" min="18" max="20" width="38.29"/>
+    <col customWidth="1" min="21" max="21" width="48.29"/>
+    <col customWidth="1" min="22" max="22" width="21.43"/>
+    <col customWidth="1" min="23" max="23" width="29.14"/>
+    <col customWidth="1" min="24" max="24" width="26.43"/>
+    <col customWidth="1" min="25" max="25" width="28.71"/>
+    <col customWidth="1" min="26" max="26" width="25.71"/>
+    <col customWidth="1" min="27" max="27" width="22.29"/>
+    <col customWidth="1" min="28" max="28" width="25.29"/>
+    <col customWidth="1" min="29" max="29" width="29.86"/>
+    <col customWidth="1" min="30" max="30" width="63.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -601,10 +613,10 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -630,90 +642,102 @@
       </c>
       <c r="AB1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="2"/>
       <c r="W2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
@@ -1718,7 +1742,7 @@
   <hyperlinks>
     <hyperlink r:id="rId1" ref="K2"/>
     <hyperlink r:id="rId2" ref="Q2"/>
-    <hyperlink r:id="rId3" ref="S2"/>
+    <hyperlink r:id="rId3" ref="U2"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Feature/hounslow ch332 update csv import to support new eligibility (#84)
* Added service eligibility fields to csv service import

* Added eligibility_ethnicity_custom column to example service import spreadsheet
</commit_message>
<xml_diff>
--- a/public/downloads/services_import_example.xlsx
+++ b/public/downloads/services_import_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">eligibility_language_custom</t>
   </si>
   <si>
+    <t xml:space="preserve">eligibility_ethnicity_custom</t>
+  </si>
+  <si>
     <t xml:space="preserve">eligibility_other_custom</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Language criteria text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethnicity criteria text</t>
   </si>
   <si>
     <t xml:space="preserve">Other criteria text</t>
@@ -338,21 +344,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD14" activeCellId="0" sqref="AD14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD2" activeCellId="0" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="61.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.14"/>
@@ -360,7 +366,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="49.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="38.29"/>
@@ -373,8 +379,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="22.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="26.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -465,104 +472,110 @@
       <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V2" s="2"/>
       <c r="W2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" s="5" t="s">
         <v>59</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>